<commit_message>
Resurrect the TMC debug port
</commit_message>
<xml_diff>
--- a/Doc/NIP涡轮驱动板BOM.xlsx
+++ b/Doc/NIP涡轮驱动板BOM.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Aeonmed_Prj\NIP\PCB\Turbo\Doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bitch\Desktop\TMC_BLDC_Hardware\Doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EB35000-EF1B-4F5E-B2D9-2B3AD09BABCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{220F2CEE-F095-4468-8728-FF052121BE27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,17 @@
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -75,9 +86,6 @@
     <t>74438367100</t>
   </si>
   <si>
-    <t>BSC027N04LS</t>
-  </si>
-  <si>
     <t>R-2512</t>
   </si>
   <si>
@@ -136,9 +144,6 @@
   </si>
   <si>
     <t>WE-MAPI SMT Power Inductor, size 5030, 10µH, 3.3A, 70.2mΩ</t>
-  </si>
-  <si>
-    <t>品牌：INFINEON，型号： BSC027N04LSG，40V，100A，ROHS</t>
   </si>
   <si>
     <t>品牌：VISHAY，型号：NTCS0603E3103FHT，10K@25℃, 1%，B=3960,ROHS</t>
@@ -599,6 +604,14 @@
   </si>
   <si>
     <t>75K±1%</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>BSC027N04LSG</t>
+  </si>
+  <si>
+    <t>品牌：INFINEON，
+型号： BSC027N04LSG，40V，139A，ROHS</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -1114,8 +1127,8 @@
   </sheetPr>
   <dimension ref="B2:F71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1144,10 +1157,10 @@
     </row>
     <row r="3" spans="2:6" ht="60.75" x14ac:dyDescent="0.15">
       <c r="B3" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="10" t="s">
         <v>111</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="11" t="s">
         <v>0</v>
@@ -1159,13 +1172,13 @@
     </row>
     <row r="4" spans="2:6" ht="60.75" x14ac:dyDescent="0.15">
       <c r="B4" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="C4" s="10" t="s">
         <v>112</v>
       </c>
-      <c r="C4" s="10" t="s">
-        <v>114</v>
-      </c>
       <c r="D4" s="11" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="12">
         <v>15</v>
@@ -1174,13 +1187,13 @@
     </row>
     <row r="5" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B5" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="12">
         <v>2</v>
@@ -1189,13 +1202,13 @@
     </row>
     <row r="6" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B6" s="9" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C6" s="10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E6" s="12">
         <v>4</v>
@@ -1207,10 +1220,10 @@
         <v>5</v>
       </c>
       <c r="C7" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E7" s="12">
         <v>2</v>
@@ -1222,10 +1235,10 @@
         <v>6</v>
       </c>
       <c r="C8" s="10" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D8" s="11" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="12">
         <v>3</v>
@@ -1234,13 +1247,13 @@
     </row>
     <row r="9" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B9" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="12">
         <v>2</v>
@@ -1252,10 +1265,10 @@
         <v>7</v>
       </c>
       <c r="C10" s="10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D10" s="11" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="E10" s="12">
         <v>3</v>
@@ -1264,13 +1277,13 @@
     </row>
     <row r="11" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B11" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E11" s="12">
         <v>3</v>
@@ -1279,13 +1292,13 @@
     </row>
     <row r="12" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B12" s="9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C12" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D12" s="11" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E12" s="12">
         <v>2</v>
@@ -1297,10 +1310,10 @@
         <v>6</v>
       </c>
       <c r="C13" s="10" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="E13" s="12">
         <v>1</v>
@@ -1312,10 +1325,10 @@
         <v>5</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D14" s="11" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E14" s="12">
         <v>1</v>
@@ -1327,10 +1340,10 @@
         <v>6</v>
       </c>
       <c r="C15" s="10" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D15" s="11" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E15" s="12">
         <v>1</v>
@@ -1342,10 +1355,10 @@
         <v>5</v>
       </c>
       <c r="C16" s="10" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D16" s="11" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E16" s="12">
         <v>1</v>
@@ -1357,10 +1370,10 @@
         <v>5</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="E17" s="12">
         <v>1</v>
@@ -1372,10 +1385,10 @@
         <v>8</v>
       </c>
       <c r="C18" s="10" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E18" s="12">
         <v>2</v>
@@ -1387,10 +1400,10 @@
         <v>9</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19" s="11" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E19" s="12">
         <v>3</v>
@@ -1402,10 +1415,10 @@
         <v>10</v>
       </c>
       <c r="C20" s="10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D20" s="11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E20" s="12">
         <v>3</v>
@@ -1414,13 +1427,13 @@
     </row>
     <row r="21" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B21" s="9" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C21" s="10" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D21" s="11" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E21" s="12">
         <v>1</v>
@@ -1432,10 +1445,10 @@
         <v>11</v>
       </c>
       <c r="C22" s="10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D22" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="E22" s="12">
         <v>1</v>
@@ -1447,10 +1460,10 @@
         <v>12</v>
       </c>
       <c r="C23" s="10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D23" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E23" s="12">
         <v>1</v>
@@ -1462,10 +1475,10 @@
         <v>13</v>
       </c>
       <c r="C24" s="10" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D24" s="11" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="E24" s="12">
         <v>1</v>
@@ -1478,7 +1491,7 @@
       </c>
       <c r="C25" s="10"/>
       <c r="D25" s="11" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E25" s="12">
         <v>1</v>
@@ -1490,10 +1503,10 @@
         <v>15</v>
       </c>
       <c r="C26" s="10" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="E26" s="12">
         <v>1</v>
@@ -1505,10 +1518,10 @@
         <v>16</v>
       </c>
       <c r="C27" s="10" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E27" s="12">
         <v>2</v>
@@ -1517,13 +1530,13 @@
     </row>
     <row r="28" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B28" s="9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C28" s="10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E28" s="12">
         <v>1</v>
@@ -1532,13 +1545,13 @@
     </row>
     <row r="29" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B29" s="9" t="s">
-        <v>17</v>
+        <v>169</v>
       </c>
       <c r="C29" s="10" t="s">
-        <v>38</v>
+        <v>170</v>
       </c>
       <c r="D29" s="11" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" s="12">
         <v>6</v>
@@ -1547,13 +1560,13 @@
     </row>
     <row r="30" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B30" s="9" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C30" s="10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="D30" s="11" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="E30" s="12">
         <v>1</v>
@@ -1562,13 +1575,13 @@
     </row>
     <row r="31" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B31" s="9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C31" s="10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="D31" s="11" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E31" s="12">
         <v>1</v>
@@ -1577,13 +1590,13 @@
     </row>
     <row r="32" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B32" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C32" s="10" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="D32" s="11" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E32" s="12">
         <v>2</v>
@@ -1592,13 +1605,13 @@
     </row>
     <row r="33" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B33" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C33" s="10" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D33" s="11" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E33" s="12">
         <v>2</v>
@@ -1607,13 +1620,13 @@
     </row>
     <row r="34" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B34" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C34" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D34" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="E34" s="12">
         <v>2</v>
@@ -1622,26 +1635,26 @@
     </row>
     <row r="35" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B35" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C35" s="10" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="D35" s="11" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="E35" s="12"/>
       <c r="F35" s="1"/>
     </row>
     <row r="36" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B36" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C36" s="10" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" s="11" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="E36" s="12">
         <v>3</v>
@@ -1650,13 +1663,13 @@
     </row>
     <row r="37" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B37" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C37" s="10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="D37" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="E37" s="12">
         <v>1</v>
@@ -1665,13 +1678,13 @@
     </row>
     <row r="38" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B38" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C38" s="10" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="E38" s="12">
         <v>10</v>
@@ -1680,13 +1693,13 @@
     </row>
     <row r="39" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B39" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E39" s="12">
         <v>1</v>
@@ -1695,13 +1708,13 @@
     </row>
     <row r="40" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B40" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D40" s="11" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E40" s="12">
         <v>2</v>
@@ -1710,13 +1723,13 @@
     </row>
     <row r="41" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B41" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C41" s="10" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D41" s="11" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E41" s="12">
         <v>2</v>
@@ -1725,13 +1738,13 @@
     </row>
     <row r="42" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B42" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C42" s="10" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D42" s="11" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E42" s="12">
         <v>3</v>
@@ -1740,13 +1753,13 @@
     </row>
     <row r="43" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B43" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C43" s="10" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D43" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E43" s="12">
         <v>4</v>
@@ -1755,13 +1768,13 @@
     </row>
     <row r="44" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B44" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C44" s="10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D44" s="11" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E44" s="12">
         <v>3</v>
@@ -1770,13 +1783,13 @@
     </row>
     <row r="45" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B45" s="9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C45" s="10" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E45" s="12">
         <v>9</v>
@@ -1785,13 +1798,13 @@
     </row>
     <row r="46" spans="2:6" ht="60.75" x14ac:dyDescent="0.15">
       <c r="B46" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C46" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E46" s="12">
         <v>17</v>
@@ -1800,13 +1813,13 @@
     </row>
     <row r="47" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B47" s="9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C47" s="10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D47" s="11" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E47" s="12">
         <v>2</v>
@@ -1815,13 +1828,13 @@
     </row>
     <row r="48" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B48" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C48" s="10" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="D48" s="11" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="E48" s="12">
         <v>1</v>
@@ -1830,13 +1843,13 @@
     </row>
     <row r="49" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B49" s="9" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C49" s="10" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D49" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="E49" s="12">
         <v>1</v>
@@ -1845,13 +1858,13 @@
     </row>
     <row r="50" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B50" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C50" s="10" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="D50" s="11" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E50" s="12">
         <v>1</v>
@@ -1860,13 +1873,13 @@
     </row>
     <row r="51" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B51" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C51" s="10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D51" s="11" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="E51" s="12">
         <v>1</v>
@@ -1875,13 +1888,13 @@
     </row>
     <row r="52" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B52" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C52" s="10" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="D52" s="11" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E52" s="12">
         <v>1</v>
@@ -1890,13 +1903,13 @@
     </row>
     <row r="53" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B53" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C53" s="10" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="D53" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E53" s="12">
         <v>1</v>
@@ -1905,13 +1918,13 @@
     </row>
     <row r="54" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B54" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="D54" s="11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E54" s="12">
         <v>1</v>
@@ -1920,13 +1933,13 @@
     </row>
     <row r="55" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B55" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D55" s="11" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="E55" s="12">
         <v>1</v>
@@ -1935,13 +1948,13 @@
     </row>
     <row r="56" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B56" s="9" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="D56" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E56" s="12">
         <v>1</v>
@@ -1950,13 +1963,13 @@
     </row>
     <row r="57" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B57" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C57" s="10" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D57" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="E57" s="12">
         <v>3</v>
@@ -1965,13 +1978,13 @@
     </row>
     <row r="58" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B58" s="9" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="D58" s="11" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E58" s="12">
         <v>2</v>
@@ -1980,13 +1993,13 @@
     </row>
     <row r="59" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B59" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C59" s="10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D59" s="11" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="E59" s="12">
         <v>1</v>
@@ -1995,13 +2008,13 @@
     </row>
     <row r="60" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B60" s="9" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D60" s="11" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E60" s="12">
         <v>2</v>
@@ -2010,13 +2023,13 @@
     </row>
     <row r="61" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B61" s="9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C61" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D61" s="11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E61" s="12">
         <v>2</v>
@@ -2025,13 +2038,13 @@
     </row>
     <row r="62" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B62" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D62" s="11" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E62" s="12">
         <v>1</v>
@@ -2040,13 +2053,13 @@
     </row>
     <row r="63" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B63" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C63" s="10" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D63" s="11" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E63" s="12">
         <v>3</v>
@@ -2055,13 +2068,13 @@
     </row>
     <row r="64" spans="2:6" ht="81" x14ac:dyDescent="0.15">
       <c r="B64" s="9" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C64" s="10" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D64" s="11" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E64" s="12">
         <v>1</v>
@@ -2070,13 +2083,13 @@
     </row>
     <row r="65" spans="2:6" ht="60.75" x14ac:dyDescent="0.15">
       <c r="B65" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C65" s="10" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D65" s="11" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E65" s="12">
         <v>1</v>
@@ -2085,13 +2098,13 @@
     </row>
     <row r="66" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B66" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C66" s="10" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D66" s="11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E66" s="12">
         <v>1</v>
@@ -2100,13 +2113,13 @@
     </row>
     <row r="67" spans="2:6" ht="20.25" x14ac:dyDescent="0.15">
       <c r="B67" s="9" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C67" s="10" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D67" s="11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E67" s="12">
         <v>1</v>
@@ -2115,13 +2128,13 @@
     </row>
     <row r="68" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B68" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C68" s="10" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D68" s="11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E68" s="12">
         <v>1</v>
@@ -2130,13 +2143,13 @@
     </row>
     <row r="69" spans="2:6" ht="40.5" x14ac:dyDescent="0.15">
       <c r="B69" s="9" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C69" s="10" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D69" s="11" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="E69" s="12">
         <v>1</v>

</xml_diff>